<commit_message>
Baixando bibliotecas no VsCode
</commit_message>
<xml_diff>
--- a/commodities_atualizado.xlsx
+++ b/commodities_atualizado.xlsx
@@ -441,10 +441,10 @@
         <v>85.31999999999999</v>
       </c>
       <c r="C2">
-        <v>85.48999999999999</v>
+        <v>84.66</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -455,7 +455,7 @@
         <v>163.59</v>
       </c>
       <c r="C3">
-        <v>162.64</v>
+        <v>158.83</v>
       </c>
       <c r="D3" t="b">
         <v>1</v>
@@ -469,7 +469,7 @@
         <v>282.2</v>
       </c>
       <c r="C4">
-        <v>276.05</v>
+        <v>277.8</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
@@ -483,7 +483,7 @@
         <v>424.37</v>
       </c>
       <c r="C5">
-        <v>393.26</v>
+        <v>386.34</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
@@ -497,10 +497,10 @@
         <v>497.76</v>
       </c>
       <c r="C6">
-        <v>498.88</v>
+        <v>482.28</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -511,7 +511,7 @@
         <v>136.23</v>
       </c>
       <c r="C7">
-        <v>134.64</v>
+        <v>134.68</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -525,10 +525,10 @@
         <v>1092.87</v>
       </c>
       <c r="C8">
-        <v>1087.87</v>
+        <v>1106.86</v>
       </c>
       <c r="D8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -539,7 +539,7 @@
         <v>321.77</v>
       </c>
       <c r="C9">
-        <v>327.99</v>
+        <v>333.47</v>
       </c>
       <c r="D9" t="b">
         <v>0</v>
@@ -553,7 +553,7 @@
         <v>1549.11</v>
       </c>
       <c r="C10">
-        <v>1546.08</v>
+        <v>1546.16</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -567,10 +567,10 @@
         <v>9.050000000000001</v>
       </c>
       <c r="C11">
-        <v>9.050000000000001</v>
+        <v>9.01</v>
       </c>
       <c r="D11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>